<commit_message>
Luận xong Huynh Đệ
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80EBEB3-7926-43FE-8A31-43B61EE89FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEEBA67-2B56-47A9-A7A5-12F966AA4FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7622" uniqueCount="3734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7640" uniqueCount="3743">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11227,6 +11227,33 @@
   </si>
   <si>
     <t>Thai Phụ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Tuế, Văn Xương, Văn Khúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tuế Phá, Tang Môn, Trực Phù đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tang Môn, Thiên Mã đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tuế Phá, Thiên Hình, Hóa Kỵ đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Phá Quân, Thiên Hình, Hóa Kỵ đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Phá Toái, Thiên Hình, Hóa Kỵ đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thái Âm đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi, Tang Môn, Tả Phù, Hữu Bật đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi, Tả Phù, Hữu Bật đồng cung tại Huynh Đệ</t>
   </si>
 </sst>
 </file>
@@ -11765,10 +11792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3812"/>
+  <dimension ref="A1:B3822"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1652" workbookViewId="0">
-      <selection activeCell="O1662" sqref="O1662"/>
+    <sheetView tabSelected="1" topLeftCell="A3794" workbookViewId="0">
+      <selection activeCell="W3805" sqref="W3805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42262,6 +42289,78 @@
       </c>
       <c r="B3812" t="s">
         <v>3612</v>
+      </c>
+    </row>
+    <row r="3814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3814" t="s">
+        <v>3734</v>
+      </c>
+      <c r="B3814" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3815" t="s">
+        <v>3735</v>
+      </c>
+      <c r="B3815" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3816" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B3816" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3817" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B3817" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3818" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B3818" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3819" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B3819" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3820" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B3820" t="s">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3821" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B3821" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3822" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B3822" t="s">
+        <v>3742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thích hoàn thiện cung huynh đệ
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3252A1FD-5467-4496-980D-3E1E30D7C136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59045673-A03B-4F56-8110-730625D05E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8840" uniqueCount="4434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8898" uniqueCount="4526">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13329,6 +13329,284 @@
   </si>
   <si>
     <t xml:space="preserve">Anh chị em qúy hiển. </t>
+  </si>
+  <si>
+    <t>Có anh trên, anh chị em đều khá giả.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Có anh trên, anh chị em thường phải xa cách nhau từ 
+lúc thiếu thời. </t>
+  </si>
+  <si>
+    <t>Tử Vi, Thiên Phủ đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Ít nhất có 3 anh em, tất cả đều quý hiển</t>
+  </si>
+  <si>
+    <t>Tử Vi, Thiên Tướng đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Bốn người trở lên, nhưng trong nhà hay có sự bất hòa vì không có sự nhường nhịn lẫn nhau, tuy vậy tất cả đều khá giả.</t>
+  </si>
+  <si>
+    <t>Tử Vi, Thất Sát đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là ba người, đều được hưởng phú qúy.</t>
+  </si>
+  <si>
+    <t>Tử Vi, Phá Quân đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiều nhất là ba người, ngoài ra còn có thêm anh chị em 
+dị bào, anh chị em sớm xa cách nhau, trong nhà thiếu hòa khí. </t>
+  </si>
+  <si>
+    <t>Tử Vi, Tham Lang đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là ba người, thường ly tán và vất vả trên đường đời</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiều nhất là hai người </t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thiên Phủ đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiều nhất là ba người, đều khá giả, nhưng không hợp tính nhau. </t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thiên Tướng đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Hai người, đều qúy hiển.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Phá Quân đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Một người, nhưng bần cùng và thường mang tật.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thất Sát đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người, thường mang tật, nên suốt đời cùng khổ, hay chết non, anh chị em bất hòa.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Tham Lang đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có hai người nhưng ly tán, cùng khổ. Trong nhà thiếu hòa khí. Anh chị em oán hận lẫn nhau, đôi khi lại còn cãi nhau.</t>
+  </si>
+  <si>
+    <t>Bốn người trở lên.</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là ba người, thường sớm xa cách nhau.</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là hai người, thường xa cách nhau từ lúc thiếu thời, có người du đãng, hoang tàng.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người nhưng cũng phiêu bạt hay cùng khổ cô đơn</t>
+  </si>
+  <si>
+    <t>Thiên Đồng, Thiên Lương đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ba người, khá giả. </t>
+  </si>
+  <si>
+    <t>Bốn hay năm người, chị em nhiều hơn anh em, tất cả đều thuận hòa và khá giả.</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là hai người, anh chị em bất hòa và xa cách nhau</t>
+  </si>
+  <si>
+    <t>Cự Môn, Thiên Đồng đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có hai người, trong nhà thiếu hòa khí, anh chị em có sớm xa cách nhau mới được toàn vẹn, có người mang cố tật hay mắc hình ngục.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai người khá giả, nhưng không hợp tính nhau. </t>
+  </si>
+  <si>
+    <t>Thiên Phủ, Vũ Khúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là ba người đều giàu có và qúy hiển.</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thiên Tướng đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là ba người, sau đều giàu có nhưng sớm xa nhau.</t>
+  </si>
+  <si>
+    <t>Phá Quân, Vũ Khúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Một người, trong nhà hay có sự xô xát, anh chị em phải xa cách nhau. </t>
+  </si>
+  <si>
+    <t>Thất Sát, Vũ Khúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Một người, nhưng mang cố tật hay bị hình thương, nếu không sớm xa cách nhau, tất bị hình khác. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sáu người trở lên, đều qúy hiển, anh em trai nhiều hơn chị em gái. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiều nhất là ba người, nhưng bất hòa. </t>
+  </si>
+  <si>
+    <t>Ba người, cũng khá giả.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có hai người, nhưng bất hòa phải xa cách nhau</t>
+  </si>
+  <si>
+    <t>Năm người, đều quý hiển</t>
+  </si>
+  <si>
+    <t>Thái Dương Thái Âm đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Năm người trở lên, tuy khá giả nhưng khiếm hòa.</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là ba người.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có hai người.</t>
+  </si>
+  <si>
+    <t>Ba người.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ Thiên Lương đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Hai người, khá giả và thuận hòa.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ Cự Môn đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Hai người, khá giả, nhưng không hợp tính nhau.</t>
+  </si>
+  <si>
+    <t>Năm người trở lên</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là bốn người, nhưng trong nhà thiếu hòa khí. Có người bị hình thương mang cố tật.</t>
+  </si>
+  <si>
+    <t>Sáu người trở lên, khá giả. Chị em gái nhiều hơn anh em trai.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có ba người, nhưng trong số đó phải có người mang cố tật, hay cùng khổ cô đơn. Anh chị em không thể chung sống với nhau lâu được.</t>
+  </si>
+  <si>
+    <t>Hai anh em</t>
+  </si>
+  <si>
+    <t>Một người</t>
+  </si>
+  <si>
+    <t>May mắn lắm mời có một người, nhưng hay chơi bời, suốt đời lang thang đây đó. Đôi khi lại có thêm nhiều anh chị em dị bào rất khá giả</t>
+  </si>
+  <si>
+    <t>Tham Lang Vũ Khúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai người, nhưng bất hòa. </t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người, nên ở riêng.  Nhưng đôi khi lại có thêm rất nhiều anh chị em dị bào.</t>
+  </si>
+  <si>
+    <t>Hai người trở lên.</t>
+  </si>
+  <si>
+    <t>Nhiều nhất là hai người.</t>
+  </si>
+  <si>
+    <t>Hai hay ba người, khá giả và thuận hòa.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiều nhất là hai người, thường xa cách nhau từ lúc thiếu thời, có người du đãng, hoang tàng. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">May mắn lắm mới có hai người, tuy khá giả nhưng khiếm hòa. </t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người, thường bị hình thương hay mang tật, trong gia đinh thiếu hòa khí.</t>
+  </si>
+  <si>
+    <t>Không có anh chị em ruột</t>
+  </si>
+  <si>
+    <t>Ba người, khá giả, nhưng khiếm hòa, sớm xa cách nhau.</t>
+  </si>
+  <si>
+    <t>May mắn lắm mới có một người nhưng cũng không thể ở gần nhau được.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May mắn lắm mới có một người phải mang cố tật, hay bất hành nhân </t>
+  </si>
+  <si>
+    <t>Kình Đà Hỏa Linh sáng tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giảm một nửa số anh chị em, trong nhà hay có sự bất hòa, thường có người mang tật. </t>
+  </si>
+  <si>
+    <t>Kình Đà Hỏa Linh tối tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Không có anh chị em, nếu có rồi cũng phải phiêu bạt, tàn lụi đến hết.</t>
+  </si>
+  <si>
+    <t>Địa Không, Địa Kiếp sáng tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Địa Không, Địa Kiếp tối tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Linh Tinh sáng tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Linh Tinh tối tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La sáng tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La tối tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Anh chị em thông minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thêm ba người, anh chị em khá giả, có danh chức và rất thông minh. </t>
+  </si>
+  <si>
+    <t>Thêm ba người, anh chị em khá giả, có danh chức và rất thông minh.</t>
   </si>
 </sst>
 </file>
@@ -13373,7 +13651,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13870,10 +14178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4422"/>
+  <dimension ref="A1:B4450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1701" workbookViewId="0">
-      <selection activeCell="A1730" sqref="A1730"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14061,8 +14369,8 @@
       <c r="A23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>162</v>
+      <c r="B23" t="s">
+        <v>4525</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -14317,8 +14625,8 @@
       <c r="A55" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>192</v>
+      <c r="B55" t="s">
+        <v>4525</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -14382,7 +14690,7 @@
         <v>200</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>200</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -14446,7 +14754,7 @@
         <v>208</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>208</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -26278,7 +26586,7 @@
         <v>27</v>
       </c>
       <c r="B1550" s="1" t="s">
-        <v>27</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="1551" spans="1:2" x14ac:dyDescent="0.25">
@@ -26358,7 +26666,7 @@
         <v>37</v>
       </c>
       <c r="B1560" s="1" t="s">
-        <v>37</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1561" spans="1:2" x14ac:dyDescent="0.25">
@@ -26998,7 +27306,7 @@
         <v>111</v>
       </c>
       <c r="B1640" s="1" t="s">
-        <v>111</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="1641" spans="1:2" x14ac:dyDescent="0.25">
@@ -27070,7 +27378,7 @@
         <v>120</v>
       </c>
       <c r="B1649" s="1" t="s">
-        <v>120</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="1650" spans="1:2" x14ac:dyDescent="0.25">
@@ -27185,6 +27493,14 @@
         <v>1662</v>
       </c>
     </row>
+    <row r="1664" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1664" s="1" t="s">
+        <v>4465</v>
+      </c>
+      <c r="B1664" s="1" t="s">
+        <v>4466</v>
+      </c>
+    </row>
     <row r="1665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1665" s="1" t="s">
         <v>1663</v>
@@ -27446,7 +27762,7 @@
         <v>1695</v>
       </c>
       <c r="B1697" s="1" t="s">
-        <v>1695</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1698" spans="1:2" x14ac:dyDescent="0.25">
@@ -27534,7 +27850,7 @@
         <v>1706</v>
       </c>
       <c r="B1708" s="1" t="s">
-        <v>1706</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1709" spans="1:2" x14ac:dyDescent="0.25">
@@ -33641,12 +33957,12 @@
         <v>3733</v>
       </c>
     </row>
-    <row r="2472" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2472" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2472" s="1" t="s">
         <v>2349</v>
       </c>
       <c r="B2472" s="1" t="s">
-        <v>2349</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="2473" spans="1:2" x14ac:dyDescent="0.25">
@@ -33693,8 +34009,8 @@
       <c r="A2478" s="1" t="s">
         <v>2355</v>
       </c>
-      <c r="B2478" s="1" t="s">
-        <v>2355</v>
+      <c r="B2478" t="s">
+        <v>4434</v>
       </c>
     </row>
     <row r="2479" spans="1:2" x14ac:dyDescent="0.25">
@@ -33742,7 +34058,7 @@
         <v>2361</v>
       </c>
       <c r="B2484" s="1" t="s">
-        <v>2361</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="2485" spans="1:2" x14ac:dyDescent="0.25">
@@ -33750,7 +34066,7 @@
         <v>2362</v>
       </c>
       <c r="B2485" s="1" t="s">
-        <v>2362</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="2486" spans="1:2" x14ac:dyDescent="0.25">
@@ -33782,7 +34098,7 @@
         <v>2366</v>
       </c>
       <c r="B2489" s="1" t="s">
-        <v>2366</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="2490" spans="1:2" x14ac:dyDescent="0.25">
@@ -33790,7 +34106,7 @@
         <v>2367</v>
       </c>
       <c r="B2490" s="1" t="s">
-        <v>2367</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="2491" spans="1:2" x14ac:dyDescent="0.25">
@@ -33798,7 +34114,7 @@
         <v>2368</v>
       </c>
       <c r="B2491" s="1" t="s">
-        <v>2368</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="2492" spans="1:2" x14ac:dyDescent="0.25">
@@ -33830,7 +34146,7 @@
         <v>2372</v>
       </c>
       <c r="B2495" s="1" t="s">
-        <v>2372</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="2496" spans="1:2" x14ac:dyDescent="0.25">
@@ -33838,7 +34154,7 @@
         <v>2373</v>
       </c>
       <c r="B2496" s="1" t="s">
-        <v>2373</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="2497" spans="1:2" x14ac:dyDescent="0.25">
@@ -33870,7 +34186,7 @@
         <v>2377</v>
       </c>
       <c r="B2500" s="1" t="s">
-        <v>2377</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2501" spans="1:2" x14ac:dyDescent="0.25">
@@ -33878,7 +34194,7 @@
         <v>2378</v>
       </c>
       <c r="B2501" s="1" t="s">
-        <v>2378</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2502" spans="1:2" x14ac:dyDescent="0.25">
@@ -33886,7 +34202,7 @@
         <v>2379</v>
       </c>
       <c r="B2502" s="1" t="s">
-        <v>2379</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2503" spans="1:2" x14ac:dyDescent="0.25">
@@ -33918,7 +34234,7 @@
         <v>2383</v>
       </c>
       <c r="B2506" s="1" t="s">
-        <v>2383</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="2507" spans="1:2" x14ac:dyDescent="0.25">
@@ -33926,7 +34242,7 @@
         <v>2384</v>
       </c>
       <c r="B2507" s="1" t="s">
-        <v>2384</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="2508" spans="1:2" x14ac:dyDescent="0.25">
@@ -33966,7 +34282,7 @@
         <v>2389</v>
       </c>
       <c r="B2512" s="1" t="s">
-        <v>2389</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="2513" spans="1:2" x14ac:dyDescent="0.25">
@@ -34014,7 +34330,7 @@
         <v>2395</v>
       </c>
       <c r="B2518" s="1" t="s">
-        <v>2395</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="2519" spans="1:2" x14ac:dyDescent="0.25">
@@ -34054,7 +34370,7 @@
         <v>2400</v>
       </c>
       <c r="B2523" s="1" t="s">
-        <v>2400</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="2524" spans="1:2" x14ac:dyDescent="0.25">
@@ -34062,15 +34378,15 @@
         <v>2401</v>
       </c>
       <c r="B2524" s="1" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="2525" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2525" s="1" t="s">
         <v>2402</v>
       </c>
       <c r="B2525" s="1" t="s">
-        <v>2402</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="2526" spans="1:2" x14ac:dyDescent="0.25">
@@ -34102,7 +34418,7 @@
         <v>2406</v>
       </c>
       <c r="B2529" s="1" t="s">
-        <v>2406</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2530" spans="1:2" x14ac:dyDescent="0.25">
@@ -34110,15 +34426,15 @@
         <v>2407</v>
       </c>
       <c r="B2530" s="1" t="s">
-        <v>2407</v>
-      </c>
-    </row>
-    <row r="2531" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2531" s="1" t="s">
         <v>2408</v>
       </c>
       <c r="B2531" s="1" t="s">
-        <v>2408</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="2532" spans="1:2" x14ac:dyDescent="0.25">
@@ -34142,7 +34458,7 @@
         <v>2411</v>
       </c>
       <c r="B2534" s="1" t="s">
-        <v>2411</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="2535" spans="1:2" x14ac:dyDescent="0.25">
@@ -34190,7 +34506,7 @@
         <v>2417</v>
       </c>
       <c r="B2540" s="1" t="s">
-        <v>2417</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="2541" spans="1:2" x14ac:dyDescent="0.25">
@@ -34225,12 +34541,12 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="2545" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2545" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2545" s="1" t="s">
         <v>2422</v>
       </c>
       <c r="B2545" s="1" t="s">
-        <v>2422</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="2546" spans="1:2" x14ac:dyDescent="0.25">
@@ -34241,12 +34557,12 @@
         <v>2423</v>
       </c>
     </row>
-    <row r="2547" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2547" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2547" s="1" t="s">
         <v>2424</v>
       </c>
       <c r="B2547" s="1" t="s">
-        <v>2424</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="2548" spans="1:2" x14ac:dyDescent="0.25">
@@ -34265,12 +34581,12 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="2550" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2550" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2550" s="1" t="s">
         <v>2427</v>
       </c>
       <c r="B2550" s="1" t="s">
-        <v>2427</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="2551" spans="1:2" x14ac:dyDescent="0.25">
@@ -34281,12 +34597,12 @@
         <v>2428</v>
       </c>
     </row>
-    <row r="2552" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2552" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2552" s="1" t="s">
         <v>2429</v>
       </c>
       <c r="B2552" s="1" t="s">
-        <v>2429</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="2553" spans="1:2" x14ac:dyDescent="0.25">
@@ -34302,7 +34618,7 @@
         <v>2431</v>
       </c>
       <c r="B2554" s="1" t="s">
-        <v>2431</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="2555" spans="1:2" x14ac:dyDescent="0.25">
@@ -34329,28 +34645,28 @@
         <v>2434</v>
       </c>
     </row>
-    <row r="2558" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2558" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2558" s="1" t="s">
         <v>2435</v>
       </c>
       <c r="B2558" s="1" t="s">
-        <v>2435</v>
-      </c>
-    </row>
-    <row r="2559" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2559" s="1" t="s">
         <v>2436</v>
       </c>
       <c r="B2559" s="1" t="s">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="2560" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2560" s="1" t="s">
         <v>2437</v>
       </c>
       <c r="B2560" s="1" t="s">
-        <v>2437</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="2561" spans="1:2" x14ac:dyDescent="0.25">
@@ -34382,7 +34698,7 @@
         <v>2441</v>
       </c>
       <c r="B2564" s="1" t="s">
-        <v>2441</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="2565" spans="1:2" x14ac:dyDescent="0.25">
@@ -34390,7 +34706,7 @@
         <v>2442</v>
       </c>
       <c r="B2565" s="1" t="s">
-        <v>2442</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="2566" spans="1:2" x14ac:dyDescent="0.25">
@@ -34398,15 +34714,15 @@
         <v>2443</v>
       </c>
       <c r="B2566" s="1" t="s">
-        <v>2443</v>
-      </c>
-    </row>
-    <row r="2567" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2567" s="1" t="s">
         <v>2444</v>
       </c>
       <c r="B2567" s="1" t="s">
-        <v>2444</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="2568" spans="1:2" x14ac:dyDescent="0.25">
@@ -34422,7 +34738,7 @@
         <v>2446</v>
       </c>
       <c r="B2569" s="1" t="s">
-        <v>2446</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="2570" spans="1:2" x14ac:dyDescent="0.25">
@@ -34438,7 +34754,7 @@
         <v>2448</v>
       </c>
       <c r="B2571" s="1" t="s">
-        <v>2448</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="2572" spans="1:2" x14ac:dyDescent="0.25">
@@ -34449,12 +34765,12 @@
         <v>2449</v>
       </c>
     </row>
-    <row r="2573" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2573" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2573" s="1" t="s">
         <v>2450</v>
       </c>
       <c r="B2573" s="1" t="s">
-        <v>2450</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="2574" spans="1:2" x14ac:dyDescent="0.25">
@@ -34470,7 +34786,7 @@
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>2452</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="2576" spans="1:2" x14ac:dyDescent="0.25">
@@ -34486,7 +34802,7 @@
         <v>2454</v>
       </c>
       <c r="B2577" s="1" t="s">
-        <v>2454</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="2578" spans="1:2" x14ac:dyDescent="0.25">
@@ -34502,7 +34818,7 @@
         <v>2456</v>
       </c>
       <c r="B2579" s="1" t="s">
-        <v>2456</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="2580" spans="1:2" x14ac:dyDescent="0.25">
@@ -34529,20 +34845,20 @@
         <v>2459</v>
       </c>
     </row>
-    <row r="2583" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2583" s="1" t="s">
         <v>2460</v>
       </c>
       <c r="B2583" s="1" t="s">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="2584" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4501</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2584" s="1" t="s">
         <v>2461</v>
       </c>
       <c r="B2584" s="1" t="s">
-        <v>2461</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="2585" spans="1:2" x14ac:dyDescent="0.25">
@@ -34550,7 +34866,7 @@
         <v>2462</v>
       </c>
       <c r="B2585" s="1" t="s">
-        <v>2462</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="2586" spans="1:2" x14ac:dyDescent="0.25">
@@ -34577,12 +34893,12 @@
         <v>2465</v>
       </c>
     </row>
-    <row r="2589" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2589" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2589" s="1" t="s">
         <v>2466</v>
       </c>
       <c r="B2589" s="1" t="s">
-        <v>2466</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="2590" spans="1:2" x14ac:dyDescent="0.25">
@@ -34590,7 +34906,7 @@
         <v>2467</v>
       </c>
       <c r="B2590" s="1" t="s">
-        <v>2467</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="2591" spans="1:2" x14ac:dyDescent="0.25">
@@ -34606,7 +34922,7 @@
         <v>2469</v>
       </c>
       <c r="B2592" s="1" t="s">
-        <v>2469</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="2593" spans="1:2" x14ac:dyDescent="0.25">
@@ -34622,7 +34938,7 @@
         <v>2471</v>
       </c>
       <c r="B2594" s="1" t="s">
-        <v>2471</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="2595" spans="1:2" x14ac:dyDescent="0.25">
@@ -34638,7 +34954,7 @@
         <v>2473</v>
       </c>
       <c r="B2596" s="1" t="s">
-        <v>2473</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="2597" spans="1:2" x14ac:dyDescent="0.25">
@@ -34654,7 +34970,7 @@
         <v>2475</v>
       </c>
       <c r="B2598" s="1" t="s">
-        <v>2475</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="2599" spans="1:2" x14ac:dyDescent="0.25">
@@ -34678,7 +34994,7 @@
         <v>2478</v>
       </c>
       <c r="B2601" s="1" t="s">
-        <v>2478</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="2602" spans="1:2" x14ac:dyDescent="0.25">
@@ -34686,7 +35002,7 @@
         <v>2479</v>
       </c>
       <c r="B2602" s="1" t="s">
-        <v>2479</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="2603" spans="1:2" x14ac:dyDescent="0.25">
@@ -34694,7 +35010,7 @@
         <v>2480</v>
       </c>
       <c r="B2603" s="1" t="s">
-        <v>2480</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="2604" spans="1:2" x14ac:dyDescent="0.25">
@@ -34721,12 +35037,12 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="2607" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2607" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2607" s="1" t="s">
         <v>2484</v>
       </c>
       <c r="B2607" s="1" t="s">
-        <v>2484</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="2608" spans="1:2" x14ac:dyDescent="0.25">
@@ -34734,7 +35050,7 @@
         <v>2485</v>
       </c>
       <c r="B2608" s="1" t="s">
-        <v>2485</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="2609" spans="1:2" x14ac:dyDescent="0.25">
@@ -34742,7 +35058,7 @@
         <v>2486</v>
       </c>
       <c r="B2609" s="1" t="s">
-        <v>2486</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="2610" spans="1:2" x14ac:dyDescent="0.25">
@@ -34769,20 +35085,20 @@
         <v>2489</v>
       </c>
     </row>
-    <row r="2613" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2613" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2613" s="1" t="s">
         <v>2490</v>
       </c>
       <c r="B2613" s="1" t="s">
-        <v>2490</v>
-      </c>
-    </row>
-    <row r="2614" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4506</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2614" s="1" t="s">
         <v>2491</v>
       </c>
       <c r="B2614" s="1" t="s">
-        <v>2491</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="2615" spans="1:2" x14ac:dyDescent="0.25">
@@ -34798,7 +35114,7 @@
         <v>2493</v>
       </c>
       <c r="B2616" s="1" t="s">
-        <v>2493</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="2617" spans="1:2" x14ac:dyDescent="0.25">
@@ -34814,7 +35130,7 @@
         <v>2495</v>
       </c>
       <c r="B2618" s="1" t="s">
-        <v>2495</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="2619" spans="1:2" x14ac:dyDescent="0.25">
@@ -34825,12 +35141,12 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="2620" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2620" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2620" s="1" t="s">
         <v>2497</v>
       </c>
       <c r="B2620" s="1" t="s">
-        <v>2497</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="2621" spans="1:2" x14ac:dyDescent="0.25">
@@ -34846,7 +35162,7 @@
         <v>2499</v>
       </c>
       <c r="B2622" s="1" t="s">
-        <v>2499</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="2623" spans="1:2" x14ac:dyDescent="0.25">
@@ -34862,7 +35178,7 @@
         <v>2501</v>
       </c>
       <c r="B2624" s="1" t="s">
-        <v>2501</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="2625" spans="1:2" x14ac:dyDescent="0.25">
@@ -34878,7 +35194,7 @@
         <v>2503</v>
       </c>
       <c r="B2626" s="1" t="s">
-        <v>2503</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2627" spans="1:2" x14ac:dyDescent="0.25">
@@ -34894,7 +35210,7 @@
         <v>2505</v>
       </c>
       <c r="B2628" s="1" t="s">
-        <v>2505</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="2629" spans="1:2" x14ac:dyDescent="0.25">
@@ -34910,7 +35226,7 @@
         <v>2507</v>
       </c>
       <c r="B2630" s="1" t="s">
-        <v>2507</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="2631" spans="1:2" x14ac:dyDescent="0.25">
@@ -34926,7 +35242,7 @@
         <v>2509</v>
       </c>
       <c r="B2632" s="1" t="s">
-        <v>2509</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2633" spans="1:2" x14ac:dyDescent="0.25">
@@ -34942,7 +35258,7 @@
         <v>2511</v>
       </c>
       <c r="B2634" s="1" t="s">
-        <v>2511</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="2635" spans="1:2" x14ac:dyDescent="0.25">
@@ -34958,7 +35274,7 @@
         <v>2513</v>
       </c>
       <c r="B2636" s="1" t="s">
-        <v>2513</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="2637" spans="1:2" x14ac:dyDescent="0.25">
@@ -36710,7 +37026,7 @@
         <v>2732</v>
       </c>
       <c r="B2855" s="1" t="s">
-        <v>2732</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="2856" spans="1:2" x14ac:dyDescent="0.25">
@@ -36758,7 +37074,7 @@
         <v>2738</v>
       </c>
       <c r="B2861" s="1" t="s">
-        <v>2738</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="2862" spans="1:2" x14ac:dyDescent="0.25">
@@ -37950,7 +38266,7 @@
         <v>2887</v>
       </c>
       <c r="B3010" s="1" t="s">
-        <v>2887</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="3011" spans="1:2" x14ac:dyDescent="0.25">
@@ -38142,7 +38458,7 @@
         <v>2911</v>
       </c>
       <c r="B3034" s="1" t="s">
-        <v>2911</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="3035" spans="1:2" x14ac:dyDescent="0.25">
@@ -39550,7 +39866,7 @@
         <v>3087</v>
       </c>
       <c r="B3210" s="1" t="s">
-        <v>3087</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="3211" spans="1:2" x14ac:dyDescent="0.25">
@@ -43758,7 +44074,7 @@
         <v>3734</v>
       </c>
       <c r="B3736" s="1" t="s">
-        <v>3734</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="3737" spans="1:2" x14ac:dyDescent="0.25">
@@ -49241,56 +49557,289 @@
         <v>4432</v>
       </c>
     </row>
+    <row r="4423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4423" s="1" t="s">
+        <v>4436</v>
+      </c>
+      <c r="B4423" s="1" t="s">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="4424" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4424" s="1" t="s">
+        <v>4438</v>
+      </c>
+      <c r="B4424" s="1" t="s">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4425" s="1" t="s">
+        <v>4440</v>
+      </c>
+      <c r="B4425" s="1" t="s">
+        <v>4441</v>
+      </c>
+    </row>
+    <row r="4426" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4426" s="1" t="s">
+        <v>4442</v>
+      </c>
+      <c r="B4426" s="1" t="s">
+        <v>4443</v>
+      </c>
+    </row>
+    <row r="4427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4427" s="1" t="s">
+        <v>4444</v>
+      </c>
+      <c r="B4427" s="1" t="s">
+        <v>4445</v>
+      </c>
+    </row>
+    <row r="4428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4428" s="1" t="s">
+        <v>4447</v>
+      </c>
+      <c r="B4428" s="1" t="s">
+        <v>4448</v>
+      </c>
+    </row>
+    <row r="4429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4429" s="1" t="s">
+        <v>4449</v>
+      </c>
+      <c r="B4429" s="1" t="s">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="4430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4430" s="1" t="s">
+        <v>4451</v>
+      </c>
+      <c r="B4430" s="1" t="s">
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="4431" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4431" s="1" t="s">
+        <v>4453</v>
+      </c>
+      <c r="B4431" s="1" t="s">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="4432" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4432" s="1" t="s">
+        <v>4455</v>
+      </c>
+      <c r="B4432" s="1" t="s">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="4433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4433" s="1" t="s">
+        <v>4461</v>
+      </c>
+      <c r="B4433" s="1" t="s">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="4434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4434" s="1" t="s">
+        <v>4468</v>
+      </c>
+      <c r="B4434" s="1" t="s">
+        <v>4469</v>
+      </c>
+    </row>
+    <row r="4435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4435" s="1" t="s">
+        <v>4470</v>
+      </c>
+      <c r="B4435" s="1" t="s">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="4436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4436" s="1" t="s">
+        <v>4471</v>
+      </c>
+      <c r="B4436" s="1" t="s">
+        <v>4472</v>
+      </c>
+    </row>
+    <row r="4437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4437" s="1" t="s">
+        <v>4473</v>
+      </c>
+      <c r="B4437" s="1" t="s">
+        <v>4474</v>
+      </c>
+    </row>
+    <row r="4438" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4438" s="1" t="s">
+        <v>4475</v>
+      </c>
+      <c r="B4438" s="1" t="s">
+        <v>4476</v>
+      </c>
+    </row>
+    <row r="4439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4439" s="1" t="s">
+        <v>4482</v>
+      </c>
+      <c r="B4439" s="1" t="s">
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="4440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4440" s="1" t="s">
+        <v>4488</v>
+      </c>
+      <c r="B4440" s="1" t="s">
+        <v>4489</v>
+      </c>
+    </row>
+    <row r="4441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4441" s="1" t="s">
+        <v>4490</v>
+      </c>
+      <c r="B4441" s="1" t="s">
+        <v>4491</v>
+      </c>
+    </row>
+    <row r="4442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4442" s="1" t="s">
+        <v>4499</v>
+      </c>
+      <c r="B4442" s="1" t="s">
+        <v>4472</v>
+      </c>
+    </row>
+    <row r="4443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4443" s="1" t="s">
+        <v>4513</v>
+      </c>
+      <c r="B4443" s="1" t="s">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4444" s="1" t="s">
+        <v>4515</v>
+      </c>
+      <c r="B4444" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4445" s="1" t="s">
+        <v>4517</v>
+      </c>
+      <c r="B4445" s="1" t="s">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4446" s="1" t="s">
+        <v>4518</v>
+      </c>
+      <c r="B4446" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4447" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4447" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B4447" s="1" t="s">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4448" s="1" t="s">
+        <v>4520</v>
+      </c>
+      <c r="B4448" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4449" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4449" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B4449" s="1" t="s">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4450" s="1" t="s">
+        <v>4522</v>
+      </c>
+      <c r="B4450" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="21" priority="92"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="19" priority="62"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="17" priority="66"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="15" priority="61"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3823 A3886:A4185 A6731:A1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="101"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="12" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3824:A3885">
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6730:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3823 A3886:A4185">
+    <cfRule type="duplicateValues" dxfId="15" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="106"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B22 A24:B54 A23 A55 A56:B1048576">
+    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B209:B1631 B1:B23 B25:B84 B143 B1805:B1809 B3442:B3823 B3886:B4185 B6731:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="11"/>
+  <conditionalFormatting sqref="B1810:B2477 B2479:B3339">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B3339">
+  <conditionalFormatting sqref="B3824:B3885">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6730:B1048576 B209:B1631 B1:B22 B25:B54 B143 B1805:B1809 B3442:B3823 B3886:B4185 B56:B84">
+    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2595">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3824:B3885">
+  <conditionalFormatting sqref="B1560">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Giải thích chính tinh nô bộc và chính tinh mệnh
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59045673-A03B-4F56-8110-730625D05E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355FB255-91D1-436A-898B-EFA7A1ED45AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8898" uniqueCount="4526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9162" uniqueCount="4663">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13607,6 +13607,417 @@
   </si>
   <si>
     <t>Thêm ba người, anh chị em khá giả, có danh chức và rất thông minh.</t>
+  </si>
+  <si>
+    <t>Cung Huynh Đệ là cung dương</t>
+  </si>
+  <si>
+    <t>Anh em trai nhiều hơn chị em gái</t>
+  </si>
+  <si>
+    <t>Cung Huynh Đệ là cung âm</t>
+  </si>
+  <si>
+    <t>Chị em gái nhiều hơn anh em trai</t>
+  </si>
+  <si>
+    <t>Sinh con trai đầu lòng mới dễ nuôi.</t>
+  </si>
+  <si>
+    <t>Sinh con gái đầu lòng mới dễ nuôi.</t>
+  </si>
+  <si>
+    <t>Con dị bào rất khá giả và hiếu thảo</t>
+  </si>
+  <si>
+    <t>Dễ có con dị bào</t>
+  </si>
+  <si>
+    <t>Chắc chắn có con nuôi hiếu thảo</t>
+  </si>
+  <si>
+    <t>Dễ sinh đôi</t>
+  </si>
+  <si>
+    <t>Thiên Phủ tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thiên Lương tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thất Sát tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Âm tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Cự Môn tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tham Lang tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Phá Quân đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Phá Quân đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thất Sát và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thất Sát và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thất Sát và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thất Sát và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thất Sát và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thất Sát và Phá Quân đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Phá Quân đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thái Dương và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thái Dương và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thái Dương và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thái Dương và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thái Dương và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thái Dương và Phá Quân đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Thái Âm đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Cự Môn đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Tham Lang đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Phá Quân đồng cung tại cung Huynh Đệ tại cung dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Phủ và Phá Quân đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Tướng và Phá Quân đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Lương và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thất Sát và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thất Sát và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thất Sát và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thất Sát và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thất Sát và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thất Sát và Phá Quân đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Đồng và Phá Quân đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thái Dương và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thái Dương và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thái Dương và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thái Dương và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thái Dương và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thái Dương và Phá Quân đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Thái Âm đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Cự Môn đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Tham Lang đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Liêm Trinh đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Vũ Khúc đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ và Phá Quân đồng cung tại cung Huynh Đệ tại cung âm</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thái Âm đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Cự Môn đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Tham Lang đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Liêm Trinh đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi  và Vũ Khúc đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi  và Phá Quân đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Phủ đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Tướng đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Lương đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thất Sát đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Đồng đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thái Dương đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Cơ đồng cung tại cung Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tam Thai, Tả Phù, Hữu Bật đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Phục Binh, Tướng Quân đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Cự Môn, Thiên Cơ đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Âm, Thiên Phúc đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Ân Quang, Thiên Quý đồng cung tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thái Âm đồng cung tại Huynh Đệ giáp Tam Thai</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thái Âm đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Cự Môn đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Tham Lang đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Liêm Trinh đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi  và Vũ Khúc đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi  và Phá Quân đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Phủ đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Tướng đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Lương đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thất Sát đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Đồng đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thái Dương đồng cung tại cung đối (Nô Bộc)</t>
+  </si>
+  <si>
+    <t>Tử Vi và Thiên Cơ đồng cung tại cung đối (Nô Bộc)</t>
   </si>
 </sst>
 </file>
@@ -13651,7 +14062,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14178,10 +14609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4450"/>
+  <dimension ref="A1:B4581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A4472" workbookViewId="0">
+      <selection activeCell="K4478" sqref="K4478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47933,1913 +48364,2975 @@
         <v>4216</v>
       </c>
     </row>
+    <row r="4219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4219" s="1" t="s">
+        <v>4217</v>
+      </c>
+      <c r="B4219" s="1" t="s">
+        <v>4217</v>
+      </c>
+    </row>
     <row r="4220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4220" s="1" t="s">
-        <v>4217</v>
+        <v>4218</v>
       </c>
       <c r="B4220" s="1" t="s">
-        <v>4217</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="4221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4221" s="1" t="s">
-        <v>4218</v>
+        <v>4219</v>
       </c>
       <c r="B4221" s="1" t="s">
-        <v>4218</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="4222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4222" s="1" t="s">
-        <v>4219</v>
+        <v>4220</v>
       </c>
       <c r="B4222" s="1" t="s">
-        <v>4219</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="4223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4223" s="1" t="s">
-        <v>4220</v>
+        <v>4221</v>
       </c>
       <c r="B4223" s="1" t="s">
-        <v>4220</v>
+        <v>4221</v>
       </c>
     </row>
     <row r="4224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4224" s="1" t="s">
-        <v>4221</v>
+        <v>4222</v>
       </c>
       <c r="B4224" s="1" t="s">
-        <v>4221</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="4225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4225" s="1" t="s">
-        <v>4222</v>
+        <v>4223</v>
       </c>
       <c r="B4225" s="1" t="s">
-        <v>4222</v>
+        <v>4223</v>
       </c>
     </row>
     <row r="4226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4226" s="1" t="s">
-        <v>4223</v>
+        <v>4224</v>
       </c>
       <c r="B4226" s="1" t="s">
-        <v>4223</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="4227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4227" s="1" t="s">
-        <v>4224</v>
+        <v>4225</v>
       </c>
       <c r="B4227" s="1" t="s">
-        <v>4224</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="4228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4228" s="1" t="s">
-        <v>4225</v>
+        <v>4226</v>
       </c>
       <c r="B4228" s="1" t="s">
-        <v>4424</v>
-      </c>
-    </row>
-    <row r="4229" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4226</v>
+      </c>
+    </row>
+    <row r="4229" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4229" s="1" t="s">
-        <v>4226</v>
+        <v>4227</v>
       </c>
       <c r="B4229" s="1" t="s">
-        <v>4226</v>
-      </c>
-    </row>
-    <row r="4230" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="4230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4230" s="1" t="s">
-        <v>4227</v>
+        <v>4228</v>
       </c>
       <c r="B4230" s="1" t="s">
-        <v>4426</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="4231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4231" s="1" t="s">
-        <v>4228</v>
+        <v>4229</v>
       </c>
       <c r="B4231" s="1" t="s">
-        <v>4228</v>
+        <v>4229</v>
       </c>
     </row>
     <row r="4232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4232" s="1" t="s">
-        <v>4229</v>
+        <v>4230</v>
       </c>
       <c r="B4232" s="1" t="s">
-        <v>4229</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="4233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4233" s="1" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
       <c r="B4233" s="1" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="4234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4234" s="1" t="s">
-        <v>4231</v>
+        <v>4232</v>
       </c>
       <c r="B4234" s="1" t="s">
-        <v>4231</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="4235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4235" s="1" t="s">
-        <v>4232</v>
+        <v>4233</v>
       </c>
       <c r="B4235" s="1" t="s">
-        <v>4232</v>
+        <v>4233</v>
       </c>
     </row>
     <row r="4236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4236" s="1" t="s">
-        <v>4233</v>
+        <v>4234</v>
       </c>
       <c r="B4236" s="1" t="s">
-        <v>4233</v>
-      </c>
-    </row>
-    <row r="4237" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4234</v>
+      </c>
+    </row>
+    <row r="4237" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4237" s="1" t="s">
-        <v>4234</v>
+        <v>4235</v>
       </c>
       <c r="B4237" s="1" t="s">
-        <v>4234</v>
-      </c>
-    </row>
-    <row r="4238" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4235</v>
+      </c>
+    </row>
+    <row r="4238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4238" s="1" t="s">
-        <v>4235</v>
+        <v>4236</v>
       </c>
       <c r="B4238" s="1" t="s">
-        <v>4235</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="4239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4239" s="1" t="s">
-        <v>4236</v>
+        <v>4237</v>
       </c>
       <c r="B4239" s="1" t="s">
-        <v>4236</v>
+        <v>4237</v>
       </c>
     </row>
     <row r="4240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4240" s="1" t="s">
-        <v>4237</v>
+        <v>4238</v>
       </c>
       <c r="B4240" s="1" t="s">
-        <v>4237</v>
-      </c>
-    </row>
-    <row r="4241" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4238</v>
+      </c>
+    </row>
+    <row r="4241" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4241" s="1" t="s">
-        <v>4238</v>
+        <v>4239</v>
       </c>
       <c r="B4241" s="1" t="s">
-        <v>4238</v>
-      </c>
-    </row>
-    <row r="4242" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4239</v>
+      </c>
+    </row>
+    <row r="4242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4242" s="1" t="s">
-        <v>4239</v>
+        <v>4240</v>
       </c>
       <c r="B4242" s="1" t="s">
-        <v>4239</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="4243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4243" s="1" t="s">
-        <v>4240</v>
+        <v>4241</v>
       </c>
       <c r="B4243" s="1" t="s">
-        <v>4240</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="4244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4244" s="1" t="s">
-        <v>4241</v>
+        <v>4242</v>
       </c>
       <c r="B4244" s="1" t="s">
-        <v>4241</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="4245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4245" s="1" t="s">
-        <v>4242</v>
+        <v>4243</v>
       </c>
       <c r="B4245" s="1" t="s">
-        <v>4242</v>
+        <v>4243</v>
       </c>
     </row>
     <row r="4246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4246" s="1" t="s">
-        <v>4243</v>
+        <v>4244</v>
       </c>
       <c r="B4246" s="1" t="s">
-        <v>4243</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="4247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4247" s="1" t="s">
-        <v>4244</v>
+        <v>4245</v>
       </c>
       <c r="B4247" s="1" t="s">
-        <v>4244</v>
+        <v>4245</v>
       </c>
     </row>
     <row r="4248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4248" s="1" t="s">
-        <v>4245</v>
+        <v>4246</v>
       </c>
       <c r="B4248" s="1" t="s">
-        <v>4245</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="4249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4249" s="1" t="s">
-        <v>4246</v>
+        <v>4247</v>
       </c>
       <c r="B4249" s="1" t="s">
-        <v>4246</v>
+        <v>4247</v>
       </c>
     </row>
     <row r="4250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4250" s="1" t="s">
-        <v>4247</v>
+        <v>4248</v>
       </c>
       <c r="B4250" s="1" t="s">
-        <v>4247</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="4251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4251" s="1" t="s">
-        <v>4248</v>
+        <v>4249</v>
       </c>
       <c r="B4251" s="1" t="s">
-        <v>4248</v>
+        <v>4249</v>
       </c>
     </row>
     <row r="4252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4252" s="1" t="s">
-        <v>4249</v>
+        <v>4250</v>
       </c>
       <c r="B4252" s="1" t="s">
-        <v>4249</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="4253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4253" s="1" t="s">
-        <v>4250</v>
+        <v>4251</v>
       </c>
       <c r="B4253" s="1" t="s">
-        <v>4250</v>
+        <v>4251</v>
       </c>
     </row>
     <row r="4254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4254" s="1" t="s">
-        <v>4251</v>
+        <v>4252</v>
       </c>
       <c r="B4254" s="1" t="s">
-        <v>4251</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="4255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4255" s="1" t="s">
-        <v>4252</v>
+        <v>4253</v>
       </c>
       <c r="B4255" s="1" t="s">
-        <v>4252</v>
+        <v>4253</v>
       </c>
     </row>
     <row r="4256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4256" s="1" t="s">
-        <v>4253</v>
+        <v>4254</v>
       </c>
       <c r="B4256" s="1" t="s">
-        <v>4253</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="4257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4257" s="1" t="s">
-        <v>4254</v>
+        <v>4255</v>
       </c>
       <c r="B4257" s="1" t="s">
-        <v>4254</v>
+        <v>4255</v>
       </c>
     </row>
     <row r="4258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4258" s="1" t="s">
-        <v>4255</v>
+        <v>4256</v>
       </c>
       <c r="B4258" s="1" t="s">
-        <v>4255</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="4259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4259" s="1" t="s">
-        <v>4256</v>
+        <v>4257</v>
       </c>
       <c r="B4259" s="1" t="s">
-        <v>4256</v>
+        <v>4257</v>
       </c>
     </row>
     <row r="4260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4260" s="1" t="s">
-        <v>4257</v>
+        <v>4258</v>
       </c>
       <c r="B4260" s="1" t="s">
-        <v>4257</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="4261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4261" s="1" t="s">
-        <v>4258</v>
+        <v>4259</v>
       </c>
       <c r="B4261" s="1" t="s">
-        <v>4258</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="4262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4262" s="1" t="s">
-        <v>4259</v>
+        <v>4260</v>
       </c>
       <c r="B4262" s="1" t="s">
-        <v>4259</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="4263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4263" s="1" t="s">
-        <v>4260</v>
+        <v>4261</v>
       </c>
       <c r="B4263" s="1" t="s">
-        <v>4260</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="4264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4264" s="1" t="s">
-        <v>4261</v>
+        <v>4262</v>
       </c>
       <c r="B4264" s="1" t="s">
-        <v>4261</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="4265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4265" s="1" t="s">
-        <v>4262</v>
+        <v>4263</v>
       </c>
       <c r="B4265" s="1" t="s">
-        <v>4262</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="4266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4266" s="1" t="s">
-        <v>4263</v>
+        <v>4264</v>
       </c>
       <c r="B4266" s="1" t="s">
-        <v>4263</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="4267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4267" s="1" t="s">
-        <v>4264</v>
+        <v>4265</v>
       </c>
       <c r="B4267" s="1" t="s">
-        <v>4264</v>
+        <v>4265</v>
       </c>
     </row>
     <row r="4268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4268" s="1" t="s">
-        <v>4265</v>
+        <v>4266</v>
       </c>
       <c r="B4268" s="1" t="s">
-        <v>4265</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="4269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4269" s="1" t="s">
-        <v>4266</v>
+        <v>4267</v>
       </c>
       <c r="B4269" s="1" t="s">
-        <v>4266</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="4270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4270" s="1" t="s">
-        <v>4267</v>
+        <v>4268</v>
       </c>
       <c r="B4270" s="1" t="s">
-        <v>4267</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="4271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4271" s="1" t="s">
-        <v>4268</v>
+        <v>4269</v>
       </c>
       <c r="B4271" s="1" t="s">
-        <v>4268</v>
+        <v>4269</v>
       </c>
     </row>
     <row r="4272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4272" s="1" t="s">
-        <v>4269</v>
+        <v>4270</v>
       </c>
       <c r="B4272" s="1" t="s">
-        <v>4269</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="4273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4273" s="1" t="s">
-        <v>4270</v>
+        <v>4271</v>
       </c>
       <c r="B4273" s="1" t="s">
-        <v>4433</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="4274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4274" s="1" t="s">
-        <v>4271</v>
+        <v>4272</v>
       </c>
       <c r="B4274" s="1" t="s">
-        <v>4271</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="4275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4275" s="1" t="s">
-        <v>4272</v>
+        <v>4273</v>
       </c>
       <c r="B4275" s="1" t="s">
-        <v>4272</v>
+        <v>4273</v>
       </c>
     </row>
     <row r="4276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4276" s="1" t="s">
-        <v>4273</v>
+        <v>4274</v>
       </c>
       <c r="B4276" s="1" t="s">
-        <v>4273</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="4277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4277" s="1" t="s">
-        <v>4274</v>
+        <v>4275</v>
       </c>
       <c r="B4277" s="1" t="s">
-        <v>4274</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="4278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4278" s="1" t="s">
-        <v>4275</v>
+        <v>4276</v>
       </c>
       <c r="B4278" s="1" t="s">
-        <v>4275</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="4279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4279" s="1" t="s">
-        <v>4276</v>
+        <v>4277</v>
       </c>
       <c r="B4279" s="1" t="s">
-        <v>4276</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="4280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4280" s="1" t="s">
-        <v>4277</v>
+        <v>4278</v>
       </c>
       <c r="B4280" s="1" t="s">
-        <v>4277</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="4281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4281" s="1" t="s">
-        <v>4278</v>
+        <v>4279</v>
       </c>
       <c r="B4281" s="1" t="s">
-        <v>4278</v>
-      </c>
-    </row>
-    <row r="4282" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="4282" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4282" s="1" t="s">
-        <v>4279</v>
+        <v>4280</v>
       </c>
       <c r="B4282" s="1" t="s">
-        <v>4279</v>
-      </c>
-    </row>
-    <row r="4283" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="4283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4283" s="1" t="s">
-        <v>4280</v>
+        <v>4281</v>
       </c>
       <c r="B4283" s="1" t="s">
-        <v>4280</v>
+        <v>4281</v>
       </c>
     </row>
     <row r="4284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4284" s="1" t="s">
-        <v>4281</v>
+        <v>4282</v>
       </c>
       <c r="B4284" s="1" t="s">
-        <v>4281</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="4285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4285" s="1" t="s">
-        <v>4282</v>
+        <v>4283</v>
       </c>
       <c r="B4285" s="1" t="s">
-        <v>4282</v>
+        <v>4283</v>
       </c>
     </row>
     <row r="4286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4286" s="1" t="s">
-        <v>4283</v>
+        <v>4284</v>
       </c>
       <c r="B4286" s="1" t="s">
-        <v>4283</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="4287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4287" s="1" t="s">
-        <v>4284</v>
+        <v>4285</v>
       </c>
       <c r="B4287" s="1" t="s">
-        <v>4284</v>
+        <v>4285</v>
       </c>
     </row>
     <row r="4288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4288" s="1" t="s">
-        <v>4285</v>
+        <v>4286</v>
       </c>
       <c r="B4288" s="1" t="s">
-        <v>4285</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="4289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4289" s="1" t="s">
-        <v>4286</v>
+        <v>4287</v>
       </c>
       <c r="B4289" s="1" t="s">
-        <v>4286</v>
+        <v>4287</v>
       </c>
     </row>
     <row r="4290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4290" s="1" t="s">
-        <v>4287</v>
+        <v>4288</v>
       </c>
       <c r="B4290" s="1" t="s">
-        <v>4287</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="4291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4291" s="1" t="s">
-        <v>4288</v>
+        <v>4289</v>
       </c>
       <c r="B4291" s="1" t="s">
-        <v>4288</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="4292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4292" s="1" t="s">
-        <v>4289</v>
+        <v>4290</v>
       </c>
       <c r="B4292" s="1" t="s">
-        <v>4289</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="4293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4293" s="1" t="s">
-        <v>4290</v>
+        <v>4291</v>
       </c>
       <c r="B4293" s="1" t="s">
-        <v>4290</v>
+        <v>4291</v>
       </c>
     </row>
     <row r="4294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4294" s="1" t="s">
-        <v>4291</v>
+        <v>4292</v>
       </c>
       <c r="B4294" s="1" t="s">
-        <v>4291</v>
-      </c>
-    </row>
-    <row r="4295" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="4295" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4295" s="1" t="s">
-        <v>4292</v>
+        <v>4293</v>
       </c>
       <c r="B4295" s="1" t="s">
-        <v>4411</v>
-      </c>
-    </row>
-    <row r="4296" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4410</v>
+      </c>
+    </row>
+    <row r="4296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4296" s="1" t="s">
-        <v>4293</v>
+        <v>4294</v>
       </c>
       <c r="B4296" s="1" t="s">
-        <v>4410</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="4297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4297" s="1" t="s">
-        <v>4294</v>
+        <v>4295</v>
       </c>
       <c r="B4297" s="1" t="s">
-        <v>4294</v>
+        <v>4295</v>
       </c>
     </row>
     <row r="4298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4298" s="1" t="s">
-        <v>4295</v>
+        <v>4429</v>
       </c>
       <c r="B4298" s="1" t="s">
-        <v>4295</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="4299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4299" s="1" t="s">
-        <v>4429</v>
+        <v>4296</v>
       </c>
       <c r="B4299" s="1" t="s">
-        <v>4430</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="4300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4300" s="1" t="s">
-        <v>4296</v>
+        <v>4297</v>
       </c>
       <c r="B4300" s="1" t="s">
-        <v>4296</v>
+        <v>4297</v>
       </c>
     </row>
     <row r="4301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4301" s="1" t="s">
-        <v>4297</v>
+        <v>4298</v>
       </c>
       <c r="B4301" s="1" t="s">
-        <v>4297</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="4302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4302" s="1" t="s">
-        <v>4298</v>
+        <v>4299</v>
       </c>
       <c r="B4302" s="1" t="s">
-        <v>4298</v>
+        <v>4299</v>
       </c>
     </row>
     <row r="4303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4303" s="1" t="s">
-        <v>4299</v>
+        <v>4300</v>
       </c>
       <c r="B4303" s="1" t="s">
-        <v>4299</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="4304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4304" s="1" t="s">
-        <v>4300</v>
+        <v>4301</v>
       </c>
       <c r="B4304" s="1" t="s">
-        <v>4300</v>
+        <v>4301</v>
       </c>
     </row>
     <row r="4305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4305" s="1" t="s">
-        <v>4301</v>
+        <v>4302</v>
       </c>
       <c r="B4305" s="1" t="s">
-        <v>4301</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="4306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4306" s="1" t="s">
-        <v>4302</v>
+        <v>4303</v>
       </c>
       <c r="B4306" s="1" t="s">
-        <v>4302</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="4307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4307" s="1" t="s">
-        <v>4303</v>
+        <v>4304</v>
       </c>
       <c r="B4307" s="1" t="s">
-        <v>4303</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="4308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4308" s="1" t="s">
-        <v>4304</v>
+        <v>4305</v>
       </c>
       <c r="B4308" s="1" t="s">
-        <v>4304</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="4309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4309" s="1" t="s">
-        <v>4305</v>
+        <v>4306</v>
       </c>
       <c r="B4309" s="1" t="s">
-        <v>4305</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="4310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4310" s="1" t="s">
-        <v>4306</v>
+        <v>4307</v>
       </c>
       <c r="B4310" s="1" t="s">
-        <v>4306</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="4311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4311" s="1" t="s">
-        <v>4307</v>
+        <v>4308</v>
       </c>
       <c r="B4311" s="1" t="s">
-        <v>4307</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="4312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4312" s="1" t="s">
-        <v>4308</v>
+        <v>4309</v>
       </c>
       <c r="B4312" s="1" t="s">
-        <v>4308</v>
+        <v>4309</v>
       </c>
     </row>
     <row r="4313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4313" s="1" t="s">
-        <v>4309</v>
+        <v>4310</v>
       </c>
       <c r="B4313" s="1" t="s">
-        <v>4309</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="4314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4314" s="1" t="s">
-        <v>4310</v>
+        <v>4311</v>
       </c>
       <c r="B4314" s="1" t="s">
-        <v>4310</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="4315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4315" s="1" t="s">
-        <v>4311</v>
+        <v>4312</v>
       </c>
       <c r="B4315" s="1" t="s">
-        <v>4311</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="4316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4316" s="1" t="s">
-        <v>4312</v>
+        <v>4313</v>
       </c>
       <c r="B4316" s="1" t="s">
-        <v>4312</v>
+        <v>4313</v>
       </c>
     </row>
     <row r="4317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4317" s="1" t="s">
-        <v>4313</v>
+        <v>4314</v>
       </c>
       <c r="B4317" s="1" t="s">
-        <v>4313</v>
+        <v>4314</v>
       </c>
     </row>
     <row r="4318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4318" s="1" t="s">
-        <v>4314</v>
+        <v>4315</v>
       </c>
       <c r="B4318" s="1" t="s">
-        <v>4314</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="4319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4319" s="1" t="s">
-        <v>4315</v>
+        <v>4316</v>
       </c>
       <c r="B4319" s="1" t="s">
-        <v>4315</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="4320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4320" s="1" t="s">
-        <v>4316</v>
+        <v>4317</v>
       </c>
       <c r="B4320" s="1" t="s">
-        <v>4316</v>
+        <v>4317</v>
       </c>
     </row>
     <row r="4321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4321" s="1" t="s">
-        <v>4317</v>
+        <v>4318</v>
       </c>
       <c r="B4321" s="1" t="s">
-        <v>4317</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="4322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4322" s="1" t="s">
-        <v>4318</v>
+        <v>4319</v>
       </c>
       <c r="B4322" s="1" t="s">
-        <v>4318</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="4323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4323" s="1" t="s">
-        <v>4319</v>
+        <v>4320</v>
       </c>
       <c r="B4323" s="1" t="s">
-        <v>4319</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="4324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4324" s="1" t="s">
-        <v>4320</v>
+        <v>4321</v>
       </c>
       <c r="B4324" s="1" t="s">
-        <v>4320</v>
+        <v>4321</v>
       </c>
     </row>
     <row r="4325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4325" s="1" t="s">
-        <v>4321</v>
+        <v>4322</v>
       </c>
       <c r="B4325" s="1" t="s">
-        <v>4321</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="4326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4326" s="1" t="s">
-        <v>4322</v>
+        <v>4323</v>
       </c>
       <c r="B4326" s="1" t="s">
-        <v>4322</v>
+        <v>4323</v>
       </c>
     </row>
     <row r="4327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4327" s="1" t="s">
-        <v>4323</v>
+        <v>4324</v>
       </c>
       <c r="B4327" s="1" t="s">
-        <v>4323</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="4328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4328" s="1" t="s">
-        <v>4324</v>
+        <v>4325</v>
       </c>
       <c r="B4328" s="1" t="s">
-        <v>4324</v>
+        <v>4325</v>
       </c>
     </row>
     <row r="4329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4329" s="1" t="s">
-        <v>4325</v>
+        <v>4326</v>
       </c>
       <c r="B4329" s="1" t="s">
-        <v>4325</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="4330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4330" s="1" t="s">
-        <v>4326</v>
+        <v>4327</v>
       </c>
       <c r="B4330" s="1" t="s">
-        <v>4326</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="4331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4331" s="1" t="s">
-        <v>4327</v>
+        <v>4328</v>
       </c>
       <c r="B4331" s="1" t="s">
-        <v>4327</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="4332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4332" s="1" t="s">
-        <v>4328</v>
+        <v>4329</v>
       </c>
       <c r="B4332" s="1" t="s">
-        <v>4328</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="4333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4333" s="1" t="s">
-        <v>4329</v>
+        <v>4330</v>
       </c>
       <c r="B4333" s="1" t="s">
-        <v>4329</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="4334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4334" s="1" t="s">
-        <v>4330</v>
+        <v>4331</v>
       </c>
       <c r="B4334" s="1" t="s">
-        <v>4330</v>
+        <v>4331</v>
       </c>
     </row>
     <row r="4335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4335" s="1" t="s">
-        <v>4331</v>
+        <v>4332</v>
       </c>
       <c r="B4335" s="1" t="s">
-        <v>4331</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="4336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4336" s="1" t="s">
-        <v>4332</v>
+        <v>4333</v>
       </c>
       <c r="B4336" s="1" t="s">
-        <v>4332</v>
+        <v>4333</v>
       </c>
     </row>
     <row r="4337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4337" s="1" t="s">
-        <v>4333</v>
+        <v>4334</v>
       </c>
       <c r="B4337" s="1" t="s">
-        <v>4333</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="4338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4338" s="1" t="s">
-        <v>4334</v>
+        <v>4335</v>
       </c>
       <c r="B4338" s="1" t="s">
-        <v>4334</v>
+        <v>4335</v>
       </c>
     </row>
     <row r="4339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4339" s="1" t="s">
-        <v>4335</v>
+        <v>4336</v>
       </c>
       <c r="B4339" s="1" t="s">
-        <v>4335</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="4340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4340" s="1" t="s">
-        <v>4336</v>
+        <v>4337</v>
       </c>
       <c r="B4340" s="1" t="s">
-        <v>4336</v>
+        <v>4337</v>
       </c>
     </row>
     <row r="4341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4341" s="1" t="s">
-        <v>4337</v>
+        <v>4338</v>
       </c>
       <c r="B4341" s="1" t="s">
-        <v>4337</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="4342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4342" s="1" t="s">
-        <v>4338</v>
+        <v>4339</v>
       </c>
       <c r="B4342" s="1" t="s">
-        <v>4338</v>
+        <v>4339</v>
       </c>
     </row>
     <row r="4343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4343" s="1" t="s">
-        <v>4339</v>
+        <v>4340</v>
       </c>
       <c r="B4343" s="1" t="s">
-        <v>4339</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="4344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4344" s="1" t="s">
-        <v>4340</v>
+        <v>4341</v>
       </c>
       <c r="B4344" s="1" t="s">
-        <v>4340</v>
+        <v>4341</v>
       </c>
     </row>
     <row r="4345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4345" s="1" t="s">
-        <v>4341</v>
+        <v>4342</v>
       </c>
       <c r="B4345" s="1" t="s">
-        <v>4341</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="4346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4346" s="1" t="s">
-        <v>4342</v>
+        <v>4343</v>
       </c>
       <c r="B4346" s="1" t="s">
-        <v>4342</v>
+        <v>4343</v>
       </c>
     </row>
     <row r="4347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4347" s="1" t="s">
-        <v>4343</v>
+        <v>4344</v>
       </c>
       <c r="B4347" s="1" t="s">
-        <v>4343</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="4348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4348" s="1" t="s">
-        <v>4344</v>
+        <v>4345</v>
       </c>
       <c r="B4348" s="1" t="s">
-        <v>4344</v>
+        <v>4345</v>
       </c>
     </row>
     <row r="4349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4349" s="1" t="s">
-        <v>4345</v>
+        <v>4346</v>
       </c>
       <c r="B4349" s="1" t="s">
-        <v>4345</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="4350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4350" s="1" t="s">
-        <v>4346</v>
+        <v>4347</v>
       </c>
       <c r="B4350" s="1" t="s">
-        <v>4346</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="4351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4351" s="1" t="s">
-        <v>4347</v>
+        <v>4348</v>
       </c>
       <c r="B4351" s="1" t="s">
-        <v>4347</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="4352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4352" s="1" t="s">
-        <v>4348</v>
+        <v>4349</v>
       </c>
       <c r="B4352" s="1" t="s">
-        <v>4348</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="4353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4353" s="1" t="s">
-        <v>4349</v>
+        <v>4350</v>
       </c>
       <c r="B4353" s="1" t="s">
-        <v>4349</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="4354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4354" s="1" t="s">
-        <v>4350</v>
+        <v>4351</v>
       </c>
       <c r="B4354" s="1" t="s">
-        <v>4350</v>
+        <v>4351</v>
       </c>
     </row>
     <row r="4355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4355" s="1" t="s">
-        <v>4351</v>
+        <v>4352</v>
       </c>
       <c r="B4355" s="1" t="s">
-        <v>4351</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="4356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4356" s="1" t="s">
-        <v>4352</v>
+        <v>4353</v>
       </c>
       <c r="B4356" s="1" t="s">
-        <v>4352</v>
+        <v>4353</v>
       </c>
     </row>
     <row r="4357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4357" s="1" t="s">
-        <v>4353</v>
+        <v>4354</v>
       </c>
       <c r="B4357" s="1" t="s">
-        <v>4353</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="4358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4358" s="1" t="s">
-        <v>4354</v>
+        <v>4355</v>
       </c>
       <c r="B4358" s="1" t="s">
-        <v>4354</v>
+        <v>4355</v>
       </c>
     </row>
     <row r="4359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4359" s="1" t="s">
-        <v>4355</v>
+        <v>4356</v>
       </c>
       <c r="B4359" s="1" t="s">
-        <v>4355</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="4360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4360" s="1" t="s">
-        <v>4356</v>
+        <v>4357</v>
       </c>
       <c r="B4360" s="1" t="s">
-        <v>4356</v>
+        <v>4357</v>
       </c>
     </row>
     <row r="4361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4361" s="1" t="s">
-        <v>4357</v>
+        <v>4358</v>
       </c>
       <c r="B4361" s="1" t="s">
-        <v>4357</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="4362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4362" s="1" t="s">
-        <v>4358</v>
+        <v>4359</v>
       </c>
       <c r="B4362" s="1" t="s">
-        <v>4358</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="4363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4363" s="1" t="s">
-        <v>4359</v>
+        <v>4360</v>
       </c>
       <c r="B4363" s="1" t="s">
-        <v>4359</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="4364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4364" s="1" t="s">
-        <v>4360</v>
+        <v>4361</v>
       </c>
       <c r="B4364" s="1" t="s">
-        <v>4360</v>
+        <v>4361</v>
       </c>
     </row>
     <row r="4365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4365" s="1" t="s">
-        <v>4361</v>
+        <v>4362</v>
       </c>
       <c r="B4365" s="1" t="s">
-        <v>4361</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="4366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4366" s="1" t="s">
-        <v>4362</v>
+        <v>4363</v>
       </c>
       <c r="B4366" s="1" t="s">
-        <v>4362</v>
+        <v>4363</v>
       </c>
     </row>
     <row r="4367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4367" s="1" t="s">
-        <v>4363</v>
+        <v>4364</v>
       </c>
       <c r="B4367" s="1" t="s">
-        <v>4363</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="4368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4368" s="1" t="s">
-        <v>4364</v>
+        <v>4365</v>
       </c>
       <c r="B4368" s="1" t="s">
-        <v>4364</v>
+        <v>4365</v>
       </c>
     </row>
     <row r="4369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4369" s="1" t="s">
-        <v>4365</v>
+        <v>4366</v>
       </c>
       <c r="B4369" s="1" t="s">
-        <v>4365</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="4370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4370" s="1" t="s">
-        <v>4366</v>
+        <v>4367</v>
       </c>
       <c r="B4370" s="1" t="s">
-        <v>4366</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="4371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4371" s="1" t="s">
-        <v>4367</v>
+        <v>4368</v>
       </c>
       <c r="B4371" s="1" t="s">
-        <v>4367</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="4372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4372" s="1" t="s">
-        <v>4368</v>
+        <v>4369</v>
       </c>
       <c r="B4372" s="1" t="s">
-        <v>4368</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="4373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4373" s="1" t="s">
-        <v>4369</v>
+        <v>4370</v>
       </c>
       <c r="B4373" s="1" t="s">
-        <v>4369</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="4374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4374" s="1" t="s">
-        <v>4370</v>
+        <v>4371</v>
       </c>
       <c r="B4374" s="1" t="s">
-        <v>4370</v>
+        <v>4371</v>
       </c>
     </row>
     <row r="4375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4375" s="1" t="s">
-        <v>4371</v>
+        <v>4372</v>
       </c>
       <c r="B4375" s="1" t="s">
-        <v>4371</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="4376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4376" s="1" t="s">
-        <v>4372</v>
+        <v>4373</v>
       </c>
       <c r="B4376" s="1" t="s">
-        <v>4372</v>
+        <v>4373</v>
       </c>
     </row>
     <row r="4377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4377" s="1" t="s">
-        <v>4373</v>
+        <v>4374</v>
       </c>
       <c r="B4377" s="1" t="s">
-        <v>4373</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="4378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4378" s="1" t="s">
-        <v>4374</v>
+        <v>4375</v>
       </c>
       <c r="B4378" s="1" t="s">
-        <v>4374</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="4379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4379" s="1" t="s">
-        <v>4375</v>
+        <v>4376</v>
       </c>
       <c r="B4379" s="1" t="s">
-        <v>4375</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="4380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4380" s="1" t="s">
-        <v>4376</v>
+        <v>4377</v>
       </c>
       <c r="B4380" s="1" t="s">
-        <v>4376</v>
+        <v>4377</v>
       </c>
     </row>
     <row r="4381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4381" s="1" t="s">
-        <v>4377</v>
+        <v>4378</v>
       </c>
       <c r="B4381" s="1" t="s">
-        <v>4377</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="4382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4382" s="1" t="s">
-        <v>4378</v>
+        <v>4379</v>
       </c>
       <c r="B4382" s="1" t="s">
-        <v>4378</v>
+        <v>4379</v>
       </c>
     </row>
     <row r="4383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4383" s="1" t="s">
-        <v>4379</v>
+        <v>4380</v>
       </c>
       <c r="B4383" s="1" t="s">
-        <v>4379</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="4384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4384" s="1" t="s">
-        <v>4380</v>
+        <v>4381</v>
       </c>
       <c r="B4384" s="1" t="s">
-        <v>4380</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="4385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4385" s="1" t="s">
-        <v>4381</v>
+        <v>4382</v>
       </c>
       <c r="B4385" s="1" t="s">
-        <v>4381</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="4386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4386" s="1" t="s">
-        <v>4382</v>
+        <v>4383</v>
       </c>
       <c r="B4386" s="1" t="s">
-        <v>4382</v>
+        <v>4383</v>
       </c>
     </row>
     <row r="4387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4387" s="1" t="s">
-        <v>4383</v>
+        <v>4384</v>
       </c>
       <c r="B4387" s="1" t="s">
-        <v>4383</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="4388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4388" s="1" t="s">
-        <v>4384</v>
+        <v>4385</v>
       </c>
       <c r="B4388" s="1" t="s">
-        <v>4384</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="4389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4389" s="1" t="s">
-        <v>4385</v>
+        <v>4386</v>
       </c>
       <c r="B4389" s="1" t="s">
-        <v>4385</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="4390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4390" s="1" t="s">
-        <v>4386</v>
+        <v>4387</v>
       </c>
       <c r="B4390" s="1" t="s">
-        <v>4386</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="4391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4391" s="1" t="s">
-        <v>4387</v>
+        <v>4388</v>
       </c>
       <c r="B4391" s="1" t="s">
-        <v>4387</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="4392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4392" s="1" t="s">
-        <v>4388</v>
+        <v>4389</v>
       </c>
       <c r="B4392" s="1" t="s">
-        <v>4388</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="4393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4393" s="1" t="s">
-        <v>4389</v>
+        <v>4390</v>
       </c>
       <c r="B4393" s="1" t="s">
-        <v>4389</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="4394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4394" s="1" t="s">
-        <v>4390</v>
+        <v>4391</v>
       </c>
       <c r="B4394" s="1" t="s">
-        <v>4390</v>
+        <v>4391</v>
       </c>
     </row>
     <row r="4395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4395" s="1" t="s">
-        <v>4391</v>
+        <v>4392</v>
       </c>
       <c r="B4395" s="1" t="s">
-        <v>4391</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="4396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4396" s="1" t="s">
-        <v>4392</v>
+        <v>4393</v>
       </c>
       <c r="B4396" s="1" t="s">
-        <v>4392</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="4397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4397" s="1" t="s">
-        <v>4393</v>
+        <v>4394</v>
       </c>
       <c r="B4397" s="1" t="s">
-        <v>4393</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="4398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4398" s="1" t="s">
-        <v>4394</v>
+        <v>4395</v>
       </c>
       <c r="B4398" s="1" t="s">
-        <v>4394</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="4399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4399" s="1" t="s">
-        <v>4395</v>
+        <v>4396</v>
       </c>
       <c r="B4399" s="1" t="s">
-        <v>4395</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="4400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4400" s="1" t="s">
-        <v>4396</v>
+        <v>4397</v>
       </c>
       <c r="B4400" s="1" t="s">
-        <v>4396</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="4401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4401" s="1" t="s">
-        <v>4397</v>
+        <v>4398</v>
       </c>
       <c r="B4401" s="1" t="s">
-        <v>4397</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="4402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4402" s="1" t="s">
-        <v>4398</v>
+        <v>4399</v>
       </c>
       <c r="B4402" s="1" t="s">
-        <v>4398</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="4403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4403" s="1" t="s">
-        <v>4399</v>
+        <v>4400</v>
       </c>
       <c r="B4403" s="1" t="s">
-        <v>4399</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="4404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4404" s="1" t="s">
-        <v>4400</v>
+        <v>4401</v>
       </c>
       <c r="B4404" s="1" t="s">
-        <v>4400</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="4405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4405" s="1" t="s">
-        <v>4401</v>
+        <v>4402</v>
       </c>
       <c r="B4405" s="1" t="s">
-        <v>4401</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="4406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4406" s="1" t="s">
-        <v>4402</v>
+        <v>4404</v>
       </c>
       <c r="B4406" s="1" t="s">
-        <v>4403</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="4407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4407" s="1" t="s">
-        <v>4404</v>
+        <v>4405</v>
       </c>
       <c r="B4407" s="1" t="s">
-        <v>4404</v>
+        <v>4406</v>
       </c>
     </row>
     <row r="4408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4408" s="1" t="s">
-        <v>4405</v>
+        <v>4407</v>
       </c>
       <c r="B4408" s="1" t="s">
-        <v>4406</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="4409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4409" s="1" t="s">
-        <v>4407</v>
+        <v>4408</v>
       </c>
       <c r="B4409" s="1" t="s">
-        <v>4407</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="4410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4410" s="1" t="s">
-        <v>4408</v>
+        <v>4412</v>
       </c>
       <c r="B4410" s="1" t="s">
-        <v>4409</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="4411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4411" s="1" t="s">
-        <v>4412</v>
+        <v>4418</v>
       </c>
       <c r="B4411" s="1" t="s">
-        <v>4412</v>
+        <v>4413</v>
       </c>
     </row>
     <row r="4412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4412" s="1" t="s">
-        <v>4418</v>
+        <v>4415</v>
       </c>
       <c r="B4412" s="1" t="s">
-        <v>4413</v>
+        <v>4414</v>
       </c>
     </row>
     <row r="4413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4413" s="1" t="s">
-        <v>4415</v>
+        <v>4416</v>
       </c>
       <c r="B4413" s="1" t="s">
-        <v>4414</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="4414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4414" s="1" t="s">
-        <v>4416</v>
+        <v>4417</v>
       </c>
       <c r="B4414" s="1" t="s">
-        <v>4416</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="4415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4415" s="1" t="s">
-        <v>4417</v>
+        <v>4420</v>
       </c>
       <c r="B4415" s="1" t="s">
-        <v>4419</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="4416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4416" s="1" t="s">
-        <v>4420</v>
+        <v>3804</v>
       </c>
       <c r="B4416" s="1" t="s">
-        <v>4421</v>
+        <v>3804</v>
       </c>
     </row>
     <row r="4417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4417" s="1" t="s">
-        <v>3804</v>
+        <v>4295</v>
       </c>
       <c r="B4417" s="1" t="s">
-        <v>3804</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="4418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4418" s="1" t="s">
-        <v>4295</v>
+        <v>3803</v>
       </c>
       <c r="B4418" s="1" t="s">
-        <v>4422</v>
+        <v>3803</v>
       </c>
     </row>
     <row r="4419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4419" s="1" t="s">
-        <v>3803</v>
+        <v>4294</v>
       </c>
       <c r="B4419" s="1" t="s">
-        <v>3803</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="4420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4420" s="1" t="s">
-        <v>4294</v>
+        <v>4427</v>
       </c>
       <c r="B4420" s="1" t="s">
-        <v>4423</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="4421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4421" s="1" t="s">
-        <v>4427</v>
+        <v>4431</v>
       </c>
       <c r="B4421" s="1" t="s">
-        <v>4428</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="4422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4422" s="1" t="s">
-        <v>4431</v>
+        <v>4436</v>
       </c>
       <c r="B4422" s="1" t="s">
-        <v>4432</v>
-      </c>
-    </row>
-    <row r="4423" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="4423" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4423" s="1" t="s">
-        <v>4436</v>
+        <v>4438</v>
       </c>
       <c r="B4423" s="1" t="s">
-        <v>4437</v>
-      </c>
-    </row>
-    <row r="4424" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4424" s="1" t="s">
-        <v>4438</v>
+        <v>4440</v>
       </c>
       <c r="B4424" s="1" t="s">
-        <v>4439</v>
-      </c>
-    </row>
-    <row r="4425" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4441</v>
+      </c>
+    </row>
+    <row r="4425" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4425" s="1" t="s">
-        <v>4440</v>
+        <v>4442</v>
       </c>
       <c r="B4425" s="1" t="s">
-        <v>4441</v>
-      </c>
-    </row>
-    <row r="4426" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4443</v>
+      </c>
+    </row>
+    <row r="4426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4426" s="1" t="s">
-        <v>4442</v>
+        <v>4444</v>
       </c>
       <c r="B4426" s="1" t="s">
-        <v>4443</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="4427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4427" s="1" t="s">
-        <v>4444</v>
+        <v>4447</v>
       </c>
       <c r="B4427" s="1" t="s">
-        <v>4445</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="4428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4428" s="1" t="s">
-        <v>4447</v>
+        <v>4449</v>
       </c>
       <c r="B4428" s="1" t="s">
-        <v>4448</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="4429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4429" s="1" t="s">
-        <v>4449</v>
+        <v>4451</v>
       </c>
       <c r="B4429" s="1" t="s">
-        <v>4450</v>
-      </c>
-    </row>
-    <row r="4430" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="4430" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4430" s="1" t="s">
-        <v>4451</v>
+        <v>4453</v>
       </c>
       <c r="B4430" s="1" t="s">
-        <v>4452</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="4431" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4431" s="1" t="s">
-        <v>4453</v>
+        <v>4455</v>
       </c>
       <c r="B4431" s="1" t="s">
-        <v>4454</v>
-      </c>
-    </row>
-    <row r="4432" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="4432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4432" s="1" t="s">
-        <v>4455</v>
+        <v>4461</v>
       </c>
       <c r="B4432" s="1" t="s">
-        <v>4456</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="4433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4433" s="1" t="s">
-        <v>4461</v>
+        <v>4468</v>
       </c>
       <c r="B4433" s="1" t="s">
-        <v>4462</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="4434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4434" s="1" t="s">
-        <v>4468</v>
+        <v>4470</v>
       </c>
       <c r="B4434" s="1" t="s">
-        <v>4469</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="4435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4435" s="1" t="s">
-        <v>4470</v>
+        <v>4471</v>
       </c>
       <c r="B4435" s="1" t="s">
-        <v>4450</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="4436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4436" s="1" t="s">
-        <v>4471</v>
+        <v>4473</v>
       </c>
       <c r="B4436" s="1" t="s">
-        <v>4472</v>
-      </c>
-    </row>
-    <row r="4437" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4474</v>
+      </c>
+    </row>
+    <row r="4437" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4437" s="1" t="s">
-        <v>4473</v>
+        <v>4475</v>
       </c>
       <c r="B4437" s="1" t="s">
-        <v>4474</v>
-      </c>
-    </row>
-    <row r="4438" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4476</v>
+      </c>
+    </row>
+    <row r="4438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4438" s="1" t="s">
-        <v>4475</v>
+        <v>4482</v>
       </c>
       <c r="B4438" s="1" t="s">
-        <v>4476</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="4439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4439" s="1" t="s">
-        <v>4482</v>
+        <v>4488</v>
       </c>
       <c r="B4439" s="1" t="s">
-        <v>4483</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="4440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4440" s="1" t="s">
-        <v>4488</v>
+        <v>4490</v>
       </c>
       <c r="B4440" s="1" t="s">
-        <v>4489</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="4441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4441" s="1" t="s">
-        <v>4490</v>
+        <v>4499</v>
       </c>
       <c r="B4441" s="1" t="s">
-        <v>4491</v>
-      </c>
-    </row>
-    <row r="4442" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4472</v>
+      </c>
+    </row>
+    <row r="4442" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4442" s="1" t="s">
-        <v>4499</v>
+        <v>4513</v>
       </c>
       <c r="B4442" s="1" t="s">
-        <v>4472</v>
-      </c>
-    </row>
-    <row r="4443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4443" s="1" t="s">
-        <v>4513</v>
+        <v>4515</v>
       </c>
       <c r="B4443" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4444" s="1" t="s">
+        <v>4517</v>
+      </c>
+      <c r="B4444" s="1" t="s">
         <v>4514</v>
       </c>
     </row>
-    <row r="4444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4444" s="1" t="s">
-        <v>4515</v>
-      </c>
-      <c r="B4444" s="1" t="s">
+    <row r="4445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4445" s="1" t="s">
+        <v>4518</v>
+      </c>
+      <c r="B4445" s="1" t="s">
         <v>4516</v>
       </c>
     </row>
-    <row r="4445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4445" s="1" t="s">
-        <v>4517</v>
-      </c>
-      <c r="B4445" s="1" t="s">
+    <row r="4446" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4446" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B4446" s="1" t="s">
         <v>4514</v>
       </c>
     </row>
-    <row r="4446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4446" s="1" t="s">
-        <v>4518</v>
-      </c>
-      <c r="B4446" s="1" t="s">
+    <row r="4447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4447" s="1" t="s">
+        <v>4520</v>
+      </c>
+      <c r="B4447" s="1" t="s">
         <v>4516</v>
       </c>
     </row>
-    <row r="4447" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4447" s="1" t="s">
-        <v>4519</v>
-      </c>
-      <c r="B4447" s="1" t="s">
+    <row r="4448" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4448" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B4448" s="1" t="s">
         <v>4514</v>
       </c>
     </row>
-    <row r="4448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4448" s="1" t="s">
-        <v>4520</v>
-      </c>
-      <c r="B4448" s="1" t="s">
+    <row r="4449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4449" s="1" t="s">
+        <v>4522</v>
+      </c>
+      <c r="B4449" s="1" t="s">
         <v>4516</v>
-      </c>
-    </row>
-    <row r="4449" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4449" s="1" t="s">
-        <v>4521</v>
-      </c>
-      <c r="B4449" s="1" t="s">
-        <v>4514</v>
       </c>
     </row>
     <row r="4450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4450" s="1" t="s">
-        <v>4522</v>
+        <v>4526</v>
       </c>
       <c r="B4450" s="1" t="s">
-        <v>4516</v>
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4451" s="1" t="s">
+        <v>4528</v>
+      </c>
+      <c r="B4451" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4452" s="1" t="s">
+        <v>4536</v>
+      </c>
+      <c r="B4452" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4453" s="1" t="s">
+        <v>4537</v>
+      </c>
+      <c r="B4453" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4454" s="1" t="s">
+        <v>4538</v>
+      </c>
+      <c r="B4454" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4455" s="1" t="s">
+        <v>4539</v>
+      </c>
+      <c r="B4455" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4456" s="1" t="s">
+        <v>4540</v>
+      </c>
+      <c r="B4456" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4457" s="1" t="s">
+        <v>4541</v>
+      </c>
+      <c r="B4457" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4458" s="1" t="s">
+        <v>4542</v>
+      </c>
+      <c r="B4458" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4459" s="1" t="s">
+        <v>4543</v>
+      </c>
+      <c r="B4459" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4460" s="1" t="s">
+        <v>4544</v>
+      </c>
+      <c r="B4460" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4461" s="1" t="s">
+        <v>4545</v>
+      </c>
+      <c r="B4461" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4462" s="1" t="s">
+        <v>4546</v>
+      </c>
+      <c r="B4462" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4463" s="1" t="s">
+        <v>4547</v>
+      </c>
+      <c r="B4463" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4464" s="1" t="s">
+        <v>4548</v>
+      </c>
+      <c r="B4464" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4465" s="1" t="s">
+        <v>4549</v>
+      </c>
+      <c r="B4465" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4466" s="1" t="s">
+        <v>4550</v>
+      </c>
+      <c r="B4466" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4467" s="1" t="s">
+        <v>4551</v>
+      </c>
+      <c r="B4467" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4468" s="1" t="s">
+        <v>4552</v>
+      </c>
+      <c r="B4468" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4469" s="1" t="s">
+        <v>4553</v>
+      </c>
+      <c r="B4469" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4470" s="1" t="s">
+        <v>4554</v>
+      </c>
+      <c r="B4470" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4471" s="1" t="s">
+        <v>4555</v>
+      </c>
+      <c r="B4471" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4472" s="1" t="s">
+        <v>4556</v>
+      </c>
+      <c r="B4472" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4473" s="1" t="s">
+        <v>4557</v>
+      </c>
+      <c r="B4473" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4474" s="1" t="s">
+        <v>4558</v>
+      </c>
+      <c r="B4474" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4475" s="1" t="s">
+        <v>4559</v>
+      </c>
+      <c r="B4475" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4476" s="1" t="s">
+        <v>4560</v>
+      </c>
+      <c r="B4476" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4477" s="1" t="s">
+        <v>4561</v>
+      </c>
+      <c r="B4477" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4478" s="1" t="s">
+        <v>4562</v>
+      </c>
+      <c r="B4478" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4479" s="1" t="s">
+        <v>4563</v>
+      </c>
+      <c r="B4479" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4480" s="1" t="s">
+        <v>4564</v>
+      </c>
+      <c r="B4480" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4481" s="1" t="s">
+        <v>4565</v>
+      </c>
+      <c r="B4481" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4482" s="1" t="s">
+        <v>4566</v>
+      </c>
+      <c r="B4482" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4483" s="1" t="s">
+        <v>4567</v>
+      </c>
+      <c r="B4483" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4484" s="1" t="s">
+        <v>4568</v>
+      </c>
+      <c r="B4484" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4485" s="1" t="s">
+        <v>4569</v>
+      </c>
+      <c r="B4485" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4486" s="1" t="s">
+        <v>4570</v>
+      </c>
+      <c r="B4486" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4487" s="1" t="s">
+        <v>4571</v>
+      </c>
+      <c r="B4487" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4488" s="1" t="s">
+        <v>4572</v>
+      </c>
+      <c r="B4488" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4489" s="1" t="s">
+        <v>4573</v>
+      </c>
+      <c r="B4489" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4490" s="1" t="s">
+        <v>4574</v>
+      </c>
+      <c r="B4490" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4491" s="1" t="s">
+        <v>4575</v>
+      </c>
+      <c r="B4491" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4492" s="1" t="s">
+        <v>4576</v>
+      </c>
+      <c r="B4492" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4493" s="1" t="s">
+        <v>4577</v>
+      </c>
+      <c r="B4493" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4494" s="1" t="s">
+        <v>4578</v>
+      </c>
+      <c r="B4494" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4495" s="1" t="s">
+        <v>4579</v>
+      </c>
+      <c r="B4495" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4496" s="1" t="s">
+        <v>4580</v>
+      </c>
+      <c r="B4496" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4497" s="1" t="s">
+        <v>4581</v>
+      </c>
+      <c r="B4497" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4498" s="1" t="s">
+        <v>4582</v>
+      </c>
+      <c r="B4498" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4499" s="1" t="s">
+        <v>4583</v>
+      </c>
+      <c r="B4499" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4500" s="1" t="s">
+        <v>4584</v>
+      </c>
+      <c r="B4500" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4501" s="1" t="s">
+        <v>4585</v>
+      </c>
+      <c r="B4501" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4502" s="1" t="s">
+        <v>4586</v>
+      </c>
+      <c r="B4502" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4503" s="1" t="s">
+        <v>4587</v>
+      </c>
+      <c r="B4503" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4504" s="1" t="s">
+        <v>4588</v>
+      </c>
+      <c r="B4504" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4505" s="1" t="s">
+        <v>4589</v>
+      </c>
+      <c r="B4505" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4506" s="1" t="s">
+        <v>4590</v>
+      </c>
+      <c r="B4506" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4507" s="1" t="s">
+        <v>4591</v>
+      </c>
+      <c r="B4507" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4508" s="1" t="s">
+        <v>4592</v>
+      </c>
+      <c r="B4508" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4509" s="1" t="s">
+        <v>4593</v>
+      </c>
+      <c r="B4509" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4510" s="1" t="s">
+        <v>4594</v>
+      </c>
+      <c r="B4510" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4511" s="1" t="s">
+        <v>4595</v>
+      </c>
+      <c r="B4511" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4512" s="1" t="s">
+        <v>4596</v>
+      </c>
+      <c r="B4512" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4513" s="1" t="s">
+        <v>4597</v>
+      </c>
+      <c r="B4513" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4514" s="1" t="s">
+        <v>4598</v>
+      </c>
+      <c r="B4514" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4515" s="1" t="s">
+        <v>4599</v>
+      </c>
+      <c r="B4515" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4516" s="1" t="s">
+        <v>4600</v>
+      </c>
+      <c r="B4516" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4517" s="1" t="s">
+        <v>4601</v>
+      </c>
+      <c r="B4517" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4518" s="1" t="s">
+        <v>4602</v>
+      </c>
+      <c r="B4518" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4519" s="1" t="s">
+        <v>4603</v>
+      </c>
+      <c r="B4519" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4520" s="1" t="s">
+        <v>4604</v>
+      </c>
+      <c r="B4520" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4521" s="1" t="s">
+        <v>4605</v>
+      </c>
+      <c r="B4521" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4522" s="1" t="s">
+        <v>4606</v>
+      </c>
+      <c r="B4522" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4523" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4523" s="1" t="s">
+        <v>4607</v>
+      </c>
+      <c r="B4523" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4524" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4524" s="1" t="s">
+        <v>4608</v>
+      </c>
+      <c r="B4524" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4525" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4525" s="1" t="s">
+        <v>4609</v>
+      </c>
+      <c r="B4525" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4526" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4526" s="1" t="s">
+        <v>4610</v>
+      </c>
+      <c r="B4526" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4527" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4527" s="1" t="s">
+        <v>4611</v>
+      </c>
+      <c r="B4527" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4528" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4528" s="1" t="s">
+        <v>4612</v>
+      </c>
+      <c r="B4528" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4529" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4529" s="1" t="s">
+        <v>4613</v>
+      </c>
+      <c r="B4529" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4530" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4530" s="1" t="s">
+        <v>4614</v>
+      </c>
+      <c r="B4530" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4531" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4531" s="1" t="s">
+        <v>4615</v>
+      </c>
+      <c r="B4531" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4532" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4532" s="1" t="s">
+        <v>4616</v>
+      </c>
+      <c r="B4532" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4533" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4533" s="1" t="s">
+        <v>4617</v>
+      </c>
+      <c r="B4533" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4534" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4534" s="1" t="s">
+        <v>4618</v>
+      </c>
+      <c r="B4534" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4535" s="1" t="s">
+        <v>4619</v>
+      </c>
+      <c r="B4535" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4536" s="1" t="s">
+        <v>4620</v>
+      </c>
+      <c r="B4536" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4537" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4537" s="1" t="s">
+        <v>4621</v>
+      </c>
+      <c r="B4537" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4538" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4538" s="1" t="s">
+        <v>4622</v>
+      </c>
+      <c r="B4538" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4539" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4539" s="1" t="s">
+        <v>4623</v>
+      </c>
+      <c r="B4539" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4540" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4540" s="1" t="s">
+        <v>4624</v>
+      </c>
+      <c r="B4540" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4541" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4541" s="1" t="s">
+        <v>4625</v>
+      </c>
+      <c r="B4541" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4542" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4542" s="1" t="s">
+        <v>4626</v>
+      </c>
+      <c r="B4542" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4543" s="1" t="s">
+        <v>4627</v>
+      </c>
+      <c r="B4543" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4544" s="1" t="s">
+        <v>4628</v>
+      </c>
+      <c r="B4544" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4545" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4545" s="1" t="s">
+        <v>4629</v>
+      </c>
+      <c r="B4545" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4546" s="1" t="s">
+        <v>4630</v>
+      </c>
+      <c r="B4546" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4547" s="1" t="s">
+        <v>4631</v>
+      </c>
+      <c r="B4547" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4548" s="1" t="s">
+        <v>4632</v>
+      </c>
+      <c r="B4548" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4549" s="1" t="s">
+        <v>4633</v>
+      </c>
+      <c r="B4549" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4550" s="1" t="s">
+        <v>4634</v>
+      </c>
+      <c r="B4550" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4551" s="1" t="s">
+        <v>4635</v>
+      </c>
+      <c r="B4551" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4552" s="1" t="s">
+        <v>4636</v>
+      </c>
+      <c r="B4552" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4553" s="1" t="s">
+        <v>4637</v>
+      </c>
+      <c r="B4553" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4554" s="1" t="s">
+        <v>4638</v>
+      </c>
+      <c r="B4554" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4555" s="1" t="s">
+        <v>4639</v>
+      </c>
+      <c r="B4555" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4556" s="1" t="s">
+        <v>4640</v>
+      </c>
+      <c r="B4556" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4557" s="1" t="s">
+        <v>4641</v>
+      </c>
+      <c r="B4557" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4558" s="1" t="s">
+        <v>4642</v>
+      </c>
+      <c r="B4558" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4559" s="1" t="s">
+        <v>4643</v>
+      </c>
+      <c r="B4559" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4560" s="1" t="s">
+        <v>4526</v>
+      </c>
+      <c r="B4560" s="1" t="s">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="4561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4561" s="1" t="s">
+        <v>4528</v>
+      </c>
+      <c r="B4561" s="1" t="s">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="4562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4562" s="1" t="s">
+        <v>4644</v>
+      </c>
+      <c r="B4562" s="1" t="s">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="4563" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4563" s="1" t="s">
+        <v>4645</v>
+      </c>
+      <c r="B4563" s="1" t="s">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="4564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4564" s="1" t="s">
+        <v>4646</v>
+      </c>
+      <c r="B4564" s="1" t="s">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="4565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4565" s="1" t="s">
+        <v>4647</v>
+      </c>
+      <c r="B4565" s="1" t="s">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="4566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4566" s="1" t="s">
+        <v>4648</v>
+      </c>
+      <c r="B4566" s="1" t="s">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="4567" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4567" s="1" t="s">
+        <v>4420</v>
+      </c>
+      <c r="B4567" s="1" t="s">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="4568" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4568" s="1" t="s">
+        <v>4649</v>
+      </c>
+      <c r="B4568" s="1" t="s">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="4569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4569" s="1" t="s">
+        <v>4650</v>
+      </c>
+      <c r="B4569" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4570" s="1" t="s">
+        <v>4651</v>
+      </c>
+      <c r="B4570" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4571" s="1" t="s">
+        <v>4652</v>
+      </c>
+      <c r="B4571" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4572" s="1" t="s">
+        <v>4653</v>
+      </c>
+      <c r="B4572" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4573" s="1" t="s">
+        <v>4654</v>
+      </c>
+      <c r="B4573" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4574" s="1" t="s">
+        <v>4655</v>
+      </c>
+      <c r="B4574" s="1" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4575" s="1" t="s">
+        <v>4656</v>
+      </c>
+      <c r="B4575" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4576" s="1" t="s">
+        <v>4657</v>
+      </c>
+      <c r="B4576" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4577" s="1" t="s">
+        <v>4658</v>
+      </c>
+      <c r="B4577" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4578" s="1" t="s">
+        <v>4659</v>
+      </c>
+      <c r="B4578" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4579" s="1" t="s">
+        <v>4660</v>
+      </c>
+      <c r="B4579" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4580" s="1" t="s">
+        <v>4661</v>
+      </c>
+      <c r="B4580" s="1" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4581" s="1" t="s">
+        <v>4662</v>
+      </c>
+      <c r="B4581" s="1" t="s">
+        <v>4527</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="24" priority="95"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="22" priority="65"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="20" priority="69"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="18" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="17" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3824:A3885">
-    <cfRule type="duplicateValues" dxfId="16" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6730:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3823 A3886:A4185">
-    <cfRule type="duplicateValues" dxfId="15" priority="104"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="106"/>
+  <conditionalFormatting sqref="A6729:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3823 A3886:A4185">
+    <cfRule type="duplicateValues" dxfId="17" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="108"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B22 A24:B54 A23 A55 A56:B1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
+  <conditionalFormatting sqref="A1:B22 A24:B54 A23 A55 A56:B4451 A4582:B1048576">
+    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1810:B2477 B2479:B3339">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3824:B3885">
     <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B2477 B2479:B3339">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3824:B3885">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6730:B1048576 B209:B1631 B1:B22 B25:B54 B143 B1805:B1809 B3442:B3823 B3886:B4185 B56:B84">
-    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="14"/>
+  <conditionalFormatting sqref="B6729:B1048576 B209:B1631 B1:B22 B25:B54 B143 B1805:B1809 B3442:B3823 B3886:B4185 B56:B84">
+    <cfRule type="duplicateValues" dxfId="5" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2595">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1560">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4461 A4462:B4581 A4452:B4460">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1560">
+  <conditionalFormatting sqref="B4461">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Giải thích anh em
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA57F036-ACE7-422C-BE1C-42EEF4D4001F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DE5810-CEDF-4F20-8F68-2FE276862F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11110,7 +11110,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11709,8 +11729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:B3528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3492" workbookViewId="0">
-      <selection activeCell="J3516" sqref="J3516"/>
+    <sheetView tabSelected="1" topLeftCell="A3468" workbookViewId="0">
+      <selection activeCell="I3474" sqref="I3474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11723,7 +11743,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>3406</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -32915,7 +32935,7 @@
         <v>2515</v>
       </c>
       <c r="B2650" s="1" t="s">
-        <v>2515</v>
+        <v>3406</v>
       </c>
     </row>
     <row r="2651" spans="1:2" x14ac:dyDescent="0.25">
@@ -39946,82 +39966,86 @@
   <autoFilter ref="A1:B3528" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="31" priority="102"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="29" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="27" priority="76"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="25" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2771:A2832">
-    <cfRule type="duplicateValues" dxfId="24" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5676:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A2671:A2770 A2833:A3132">
-    <cfRule type="duplicateValues" dxfId="23" priority="111"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3529:B1048576 A1:B22 A24:B54 A23 A55 A56:B1980 A1981 A1982:B3398">
-    <cfRule type="duplicateValues" dxfId="21" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="20" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="18" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2771:B2832">
-    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5676:B1048576 B209:B1631 B1:B22 B25:B54 B143 B1805:B1809 B2671:B2770 B2833:B3132 B56:B84">
-    <cfRule type="duplicateValues" dxfId="12" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2589">
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1560">
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3408 A3409:B3528 A3399:B3407">
     <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1560">
+  <conditionalFormatting sqref="B3408">
     <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3408 A3409:B3528 A3399:B3407">
-    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3408">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+  <conditionalFormatting sqref="B1981">
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1981">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1981">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2786">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3154">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2473:B2665 B1810:B1980 B1982:B2471">
-    <cfRule type="duplicateValues" dxfId="1" priority="1902"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1904"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A2665">
-    <cfRule type="duplicateValues" dxfId="0" priority="1905"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1907"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2650">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>